<commit_message>
Fixed the 0208 display name and regex
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.8.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.8.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9829C12-54A8-410E-8EA3-6987A8A78951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66423DD3-E008-42F1-BAE6-E0910E8166A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1475,14 +1475,6 @@
     <t>7</t>
   </si>
   <si>
-    <t>The identification number can be displayed in the following ways:
-For enterprise numbers:
-- a group of four digits, then two groups of three digits, each group separated by a dot. Example: 1234.456.789
-- one digit, then three groups of three digits, each separated by a dot. Example: 1.234.456.789
-For establishment unit numbers:
-- one digit, then three groups of three digits, each separated by a dot. Example: 2.123.456.789</t>
-  </si>
-  <si>
     <t>BE:EN</t>
   </si>
   <si>
@@ -1960,6 +1952,11 @@
   </si>
   <si>
     <t>8.6</t>
+  </si>
+  <si>
+    <t>RegEx: [01][0-9]{9}
+Check digit: mod97
+See https://github.com/arthurdejong/python-stdnum/blob/master/stdnum/be/vat.py</t>
   </si>
 </sst>
 </file>
@@ -2749,10 +2746,10 @@
   <dimension ref="A1:AMN101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I94" sqref="I94"/>
+      <selection pane="bottomRight" activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2792,16 +2789,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>489</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>490</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>498</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>499</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>5</v>
@@ -2810,16 +2807,16 @@
         <v>6</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>428</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>429</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -2842,7 +2839,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>366</v>
@@ -2854,13 +2851,13 @@
         <v>387</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -2883,7 +2880,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>367</v>
@@ -2895,10 +2892,10 @@
         <v>388</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2921,7 +2918,7 @@
         <v>25</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>368</v>
@@ -2933,10 +2930,10 @@
         <v>389</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -2959,7 +2956,7 @@
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>369</v>
@@ -2971,13 +2968,13 @@
         <v>390</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>402</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -3000,7 +2997,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>370</v>
@@ -3012,13 +3009,13 @@
         <v>391</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>403</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -3041,7 +3038,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J7" s="9" t="s">
         <v>48</v>
@@ -3053,13 +3050,13 @@
         <v>392</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>404</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="195" x14ac:dyDescent="0.25">
@@ -3082,7 +3079,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>371</v>
@@ -3091,10 +3088,10 @@
         <v>32</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="180" x14ac:dyDescent="0.25">
@@ -3117,7 +3114,7 @@
         <v>13</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>372</v>
@@ -3126,13 +3123,13 @@
         <v>32</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>405</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="210" x14ac:dyDescent="0.25">
@@ -3155,7 +3152,7 @@
         <v>58</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>373</v>
@@ -3164,13 +3161,13 @@
         <v>32</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N10" s="7" t="s">
         <v>406</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -3193,7 +3190,7 @@
         <v>63</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>64</v>
@@ -3205,7 +3202,7 @@
         <v>407</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -3228,7 +3225,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>73</v>
@@ -3240,7 +3237,7 @@
         <v>408</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -3263,7 +3260,7 @@
         <v>13</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>127</v>
@@ -3275,7 +3272,7 @@
         <v>408</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="240" x14ac:dyDescent="0.25">
@@ -3298,7 +3295,7 @@
         <v>79</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>374</v>
@@ -3310,13 +3307,13 @@
         <v>393</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="N14" s="7" t="s">
         <v>409</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -3339,7 +3336,7 @@
         <v>79</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>339</v>
@@ -3348,13 +3345,13 @@
         <v>338</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="N15" s="7" t="s">
         <v>342</v>
       </c>
       <c r="O15" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -3377,7 +3374,7 @@
         <v>84</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>375</v>
@@ -3386,42 +3383,42 @@
         <v>383</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="17" spans="1:15 1028:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="E17" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="G17" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>505</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>506</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>32</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="18" spans="1:15 1028:1028" ht="150" x14ac:dyDescent="0.25">
@@ -3444,7 +3441,7 @@
         <v>89</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>376</v>
@@ -3456,13 +3453,13 @@
         <v>394</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="N18" s="7" t="s">
         <v>410</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="19" spans="1:15 1028:1028" ht="225" x14ac:dyDescent="0.25">
@@ -3485,7 +3482,7 @@
         <v>89</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>377</v>
@@ -3497,13 +3494,13 @@
         <v>395</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="N19" s="7" t="s">
         <v>411</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:15 1028:1028" ht="60" x14ac:dyDescent="0.25">
@@ -3526,7 +3523,7 @@
         <v>89</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J20" s="9" t="s">
         <v>100</v>
@@ -3538,10 +3535,10 @@
         <v>396</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="21" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
@@ -3564,7 +3561,7 @@
         <v>106</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J21" s="9" t="s">
         <v>107</v>
@@ -3573,10 +3570,10 @@
         <v>32</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="22" spans="1:15 1028:1028" ht="105" x14ac:dyDescent="0.25">
@@ -3599,7 +3596,7 @@
         <v>63</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>378</v>
@@ -3608,13 +3605,13 @@
         <v>385</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="N22" s="7" t="s">
         <v>412</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="23" spans="1:15 1028:1028" ht="105" x14ac:dyDescent="0.25">
@@ -3637,7 +3634,7 @@
         <v>63</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J23" s="9" t="s">
         <v>379</v>
@@ -3646,10 +3643,10 @@
         <v>386</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="O23" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="24" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
@@ -3672,7 +3669,7 @@
         <v>79</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J24" s="9" t="s">
         <v>348</v>
@@ -3681,10 +3678,10 @@
         <v>349</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="25" spans="1:15 1028:1028" ht="409.5" x14ac:dyDescent="0.25">
@@ -3707,7 +3704,7 @@
         <v>79</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>380</v>
@@ -3716,10 +3713,10 @@
         <v>353</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="26" spans="1:15 1028:1028" ht="90" x14ac:dyDescent="0.25">
@@ -3742,7 +3739,7 @@
         <v>79</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J26" s="9" t="s">
         <v>123</v>
@@ -3754,10 +3751,10 @@
         <v>397</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="27" spans="1:15 1028:1028" ht="30" x14ac:dyDescent="0.25">
@@ -3780,7 +3777,7 @@
         <v>359</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J27" s="9" t="s">
         <v>360</v>
@@ -3790,13 +3787,13 @@
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="N27" s="7" t="s">
         <v>361</v>
       </c>
       <c r="O27" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN27" s="7"/>
     </row>
@@ -3811,7 +3808,7 @@
         <v>226</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>364</v>
@@ -3820,64 +3817,64 @@
         <v>359</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="K28" s="9" t="s">
         <v>365</v>
       </c>
       <c r="L28" s="11"/>
       <c r="M28" s="11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN28" s="7"/>
     </row>
     <row r="29" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>531</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>532</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D29" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J29" s="9" t="s">
         <v>533</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>471</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>530</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>534</v>
       </c>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
       <c r="N29" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="O29" s="10" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AMN29" s="7"/>
     </row>
-    <row r="30" spans="1:15 1028:1028" ht="165" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15 1028:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>422</v>
@@ -3895,355 +3892,355 @@
         <v>425</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>426</v>
+        <v>383</v>
       </c>
       <c r="L30" s="11"/>
       <c r="M30" s="10" t="s">
-        <v>457</v>
+        <v>554</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN30" s="7"/>
     </row>
     <row r="31" spans="1:15 1028:1028" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>463</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="F31" s="12" t="s">
+      <c r="G31" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>464</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>465</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L31" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN31" s="7"/>
     </row>
     <row r="32" spans="1:15 1028:1028" ht="255" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D32" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>471</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>464</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>472</v>
       </c>
       <c r="L32" s="11"/>
       <c r="M32" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN32" s="7"/>
     </row>
     <row r="33" spans="1:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L33" s="11"/>
       <c r="M33" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="O33" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN33" s="7"/>
     </row>
     <row r="34" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="B34" s="7" t="s">
         <v>475</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>476</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J34" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>464</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J34" s="9" t="s">
+      <c r="K34" s="9" t="s">
         <v>481</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>482</v>
       </c>
       <c r="L34" s="11"/>
       <c r="M34" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN34" s="7"/>
     </row>
     <row r="35" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>477</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>478</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>463</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J35" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="E35" s="7" t="s">
-        <v>480</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>464</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J35" s="9" t="s">
+      <c r="K35" s="9" t="s">
         <v>485</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>486</v>
       </c>
       <c r="L35" s="11"/>
       <c r="M35" s="10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN35" s="7"/>
     </row>
     <row r="36" spans="1:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>507</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>508</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>509</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="F36" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J36" s="9" t="s">
         <v>510</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>501</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>511</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L36" s="11"/>
       <c r="M36" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN36" s="7"/>
     </row>
     <row r="37" spans="1:1028" ht="240" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>514</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>515</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D37" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>516</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="F37" s="12" t="s">
+        <v>500</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J37" s="9" t="s">
         <v>517</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>501</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>518</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L37" s="11"/>
       <c r="M37" s="10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="O37" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN37" s="7"/>
     </row>
     <row r="38" spans="1:1028" ht="180" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>548</v>
       </c>
-      <c r="C38" s="7" t="s">
-        <v>500</v>
-      </c>
-      <c r="D38" s="7" t="s">
+      <c r="E38" s="7" t="s">
         <v>549</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="12" t="s">
+        <v>543</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J38" s="9" t="s">
         <v>550</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>544</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J38" s="9" t="s">
-        <v>551</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L38" s="11"/>
       <c r="N38" s="7" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN38" s="7"/>
     </row>
     <row r="39" spans="1:1028" ht="90" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B39" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>540</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="D39" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="E39" s="7" t="s">
         <v>542</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="12" t="s">
         <v>543</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="G39" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="J39" s="9" t="s">
         <v>544</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>545</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L39" s="11"/>
       <c r="N39" s="7" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="O39" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="AMN39" s="7"/>
     </row>
@@ -4267,10 +4264,10 @@
         <v>13</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I40" s="18">
         <v>45260</v>
@@ -4287,7 +4284,7 @@
         <v>413</v>
       </c>
       <c r="O40" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P40" s="15"/>
       <c r="Q40" s="15"/>
@@ -5322,10 +5319,10 @@
         <v>13</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I41" s="18">
         <v>45260</v>
@@ -5336,11 +5333,11 @@
         <v>398</v>
       </c>
       <c r="M41" s="17" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="N41" s="15"/>
       <c r="O41" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
@@ -6375,10 +6372,10 @@
         <v>13</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I42" s="18">
         <v>45260</v>
@@ -6389,11 +6386,11 @@
         <v>134</v>
       </c>
       <c r="M42" s="17" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="N42" s="15"/>
       <c r="O42" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
@@ -7428,10 +7425,10 @@
         <v>13</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I43" s="18">
         <v>45260</v>
@@ -7446,7 +7443,7 @@
         <v>414</v>
       </c>
       <c r="O43" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
@@ -8479,27 +8476,27 @@
         <v>13</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I44" s="18">
         <v>45070</v>
       </c>
       <c r="J44" s="19" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K44" s="19"/>
       <c r="L44" s="17" t="s">
         <v>141</v>
       </c>
       <c r="M44" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="N44" s="15"/>
       <c r="O44" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
@@ -9534,10 +9531,10 @@
         <v>13</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I45" s="18">
         <v>45070</v>
@@ -9548,13 +9545,13 @@
         <v>399</v>
       </c>
       <c r="M45" s="17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="N45" s="15" t="s">
         <v>415</v>
       </c>
       <c r="O45" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
@@ -10589,10 +10586,10 @@
         <v>13</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I46" s="18">
         <v>45070</v>
@@ -10603,13 +10600,13 @@
       <c r="K46" s="19"/>
       <c r="L46" s="17"/>
       <c r="M46" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="O46" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
@@ -11644,7 +11641,7 @@
         <v>13</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H47" s="8" t="s">
         <v>150</v>
@@ -11653,13 +11650,13 @@
         <v>155</v>
       </c>
       <c r="M47" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="N47" s="7" t="s">
         <v>416</v>
       </c>
       <c r="O47" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="48" spans="1:1028" ht="90" x14ac:dyDescent="0.25">
@@ -11679,13 +11676,13 @@
         <v>13</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="M48" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="O48" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="49" spans="1:1027" ht="75" x14ac:dyDescent="0.25">
@@ -11706,7 +11703,7 @@
         <v>13</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H49" s="8" t="s">
         <v>150</v>
@@ -11715,13 +11712,13 @@
         <v>159</v>
       </c>
       <c r="M49" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="N49" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="O49" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="50" spans="1:1027" x14ac:dyDescent="0.25">
@@ -11744,13 +11741,13 @@
         <v>13</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="N50" s="7" t="s">
         <v>417</v>
       </c>
       <c r="O50" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="51" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
@@ -11770,13 +11767,13 @@
         <v>13</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L51" s="10" t="s">
         <v>168</v>
       </c>
       <c r="O51" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="52" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
@@ -11797,19 +11794,19 @@
         <v>13</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>400</v>
       </c>
       <c r="M52" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="N52" s="7" t="s">
         <v>418</v>
       </c>
       <c r="O52" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="53" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
@@ -11829,13 +11826,13 @@
         <v>13</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H53" s="8" t="s">
         <v>176</v>
       </c>
       <c r="O53" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="54" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
@@ -11855,7 +11852,7 @@
         <v>13</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H54" s="8" t="s">
         <v>63</v>
@@ -11867,13 +11864,13 @@
         <v>386</v>
       </c>
       <c r="M54" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="N54" s="7" t="s">
         <v>180</v>
       </c>
       <c r="O54" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="55" spans="1:1027" ht="75" x14ac:dyDescent="0.25">
@@ -11896,13 +11893,13 @@
         <v>183</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J55" s="9" t="s">
         <v>381</v>
       </c>
       <c r="O55" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="56" spans="1:1027" x14ac:dyDescent="0.25">
@@ -11923,7 +11920,7 @@
         <v>176</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J56" s="9" t="s">
         <v>187</v>
@@ -11932,7 +11929,7 @@
         <v>419</v>
       </c>
       <c r="O56" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="57" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
@@ -11955,10 +11952,10 @@
         <v>176</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O57" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="58" spans="1:1027" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -11981,7 +11978,7 @@
         <v>150</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H58" s="21" t="s">
         <v>359</v>
@@ -11997,7 +11994,7 @@
         <v>420</v>
       </c>
       <c r="O58" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P58" s="15"/>
       <c r="Q58" s="15"/>
@@ -13030,10 +13027,10 @@
         <v>150</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O59" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="60" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13054,10 +13051,10 @@
         <v>150</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O60" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="61" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13078,10 +13075,10 @@
         <v>150</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O61" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="62" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13102,10 +13099,10 @@
         <v>150</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O62" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="63" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13126,10 +13123,10 @@
         <v>150</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O63" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="64" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13150,10 +13147,10 @@
         <v>150</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O64" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
@@ -13173,10 +13170,10 @@
         <v>150</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O65" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
@@ -13197,10 +13194,10 @@
         <v>150</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O66" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
@@ -13221,10 +13218,10 @@
         <v>150</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O67" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
@@ -13245,10 +13242,10 @@
         <v>150</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O68" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
@@ -13269,10 +13266,10 @@
         <v>150</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O69" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
@@ -13293,10 +13290,10 @@
         <v>150</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O70" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
@@ -13317,10 +13314,10 @@
         <v>150</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O71" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
@@ -13341,10 +13338,10 @@
         <v>150</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O72" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
@@ -13365,10 +13362,10 @@
         <v>150</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O73" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
@@ -13389,10 +13386,10 @@
         <v>150</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O74" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
@@ -13413,10 +13410,10 @@
         <v>150</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O75" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
@@ -13437,10 +13434,10 @@
         <v>150</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O76" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
@@ -13461,10 +13458,10 @@
         <v>150</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O77" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
@@ -13485,10 +13482,10 @@
         <v>150</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O78" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -13509,10 +13506,10 @@
         <v>150</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O79" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
@@ -13533,10 +13530,10 @@
         <v>150</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O80" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="81" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13557,10 +13554,10 @@
         <v>150</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O81" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="82" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13581,10 +13578,10 @@
         <v>150</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O82" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="83" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13605,10 +13602,10 @@
         <v>150</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O83" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="84" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13629,11 +13626,11 @@
         <v>150</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I84" s="3"/>
       <c r="O84" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="85" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13654,11 +13651,11 @@
         <v>150</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I85" s="3"/>
       <c r="O85" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="86" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13679,11 +13676,11 @@
         <v>150</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I86" s="3"/>
       <c r="O86" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="87" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13704,10 +13701,10 @@
         <v>150</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O87" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="88" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13727,10 +13724,10 @@
         <v>150</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O88" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="89" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13751,11 +13748,11 @@
         <v>150</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I89" s="4"/>
       <c r="O89" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="90" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
@@ -13776,10 +13773,10 @@
         <v>150</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O90" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="91" spans="1:1027" x14ac:dyDescent="0.25">
@@ -13799,7 +13796,7 @@
         <v>320</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="H91" s="8" t="s">
         <v>89</v>
@@ -13809,7 +13806,7 @@
         <v>321</v>
       </c>
       <c r="O91" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="92" spans="1:1027" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -13830,10 +13827,10 @@
         <v>325</v>
       </c>
       <c r="G92" s="17" t="s">
+        <v>528</v>
+      </c>
+      <c r="H92" s="16" t="s">
         <v>529</v>
-      </c>
-      <c r="H92" s="16" t="s">
-        <v>530</v>
       </c>
       <c r="I92" s="22">
         <v>45138</v>
@@ -13844,7 +13841,7 @@
       <c r="M92" s="17"/>
       <c r="N92" s="15"/>
       <c r="O92" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P92" s="15"/>
       <c r="Q92" s="15"/>
@@ -14879,10 +14876,10 @@
         <v>84</v>
       </c>
       <c r="G93" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H93" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I93" s="22">
         <v>45291</v>
@@ -14895,11 +14892,11 @@
         <v>401</v>
       </c>
       <c r="M93" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="N93" s="15"/>
       <c r="O93" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P93" s="15"/>
       <c r="Q93" s="15"/>
@@ -15931,10 +15928,10 @@
         <v>84</v>
       </c>
       <c r="G94" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O94" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="95" spans="1:1027" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -15948,14 +15945,14 @@
         <v>226</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E95" s="15"/>
       <c r="F95" s="16" t="s">
         <v>106</v>
       </c>
       <c r="G95" s="17" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="H95" s="16" t="s">
         <v>359</v>
@@ -15971,7 +15968,7 @@
         <v>421</v>
       </c>
       <c r="O95" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="P95" s="15"/>
       <c r="Q95" s="15"/>
@@ -16988,25 +16985,25 @@
     </row>
     <row r="96" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="B96" s="7" t="s">
         <v>521</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="C96" s="7" t="s">
         <v>522</v>
       </c>
-      <c r="C96" s="7" t="s">
+      <c r="D96" s="7" t="s">
         <v>523</v>
       </c>
-      <c r="D96" s="7" t="s">
-        <v>524</v>
-      </c>
       <c r="F96" s="8" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O96" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="101" spans="9:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Danish PI Schemes; TICC-317
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.8.xlsx
+++ b/work-in-progress/Peppol Code Lists - Participant identifier schemes v8.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936AB3C6-D1D5-48AD-9F98-1F47F773598F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAE61C1-CE7E-42E3-BA75-EF4A1223CCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="565">
   <si>
     <t>Scheme ID</t>
   </si>
@@ -195,12 +195,6 @@
   </si>
   <si>
     <t>DK</t>
-  </si>
-  <si>
-    <t>DANISH CHAMBER OF COMMERCE Scheme</t>
-  </si>
-  <si>
-    <t>Danish Chamber of Commerce</t>
   </si>
   <si>
     <t>1) 13 digits including check digits, 2) None</t>
@@ -307,9 +301,6 @@
   </si>
   <si>
     <t>0184</t>
-  </si>
-  <si>
-    <t>DIGSTORG</t>
   </si>
   <si>
     <t>1.2.1</t>
@@ -1127,9 +1118,6 @@
     <t>0198</t>
   </si>
   <si>
-    <t>ERSTORG</t>
-  </si>
-  <si>
     <t>DK:ERST</t>
   </si>
   <si>
@@ -1212,16 +1200,6 @@
   <si>
     <t>1) Eight identification digits and a check digit. A two digit prefix will be added in the future but it will not be used to calculate the check digit.
 2) The Organization name is not part of the D-U-N-S number.</t>
-  </si>
-  <si>
-    <t>Character repertoire: the EDI identifier consists of digits only.
-The identifier has a fixed length. No separators are required.
-Structure: [123] [123456] [123456] [12], 17, &lt; &gt;, A B C D
-A: numerical value allocated by the RA to the regional sub-authority, (3 digits)
-B: numerical value allocated by the sub-authority to the registered organization (mandatory part of the identifier; 6 digits)
-C: numerical value used by the registered organization (free part; 6 digits)
-D: numerical check digit calculated by the registered organization; (2 digits)
-Check digit computation: The check digit is modular 97 computed on ABC as one number.</t>
   </si>
   <si>
     <t>Character repertoire: The EDI identifier consists of digits only.
@@ -1251,9 +1229,6 @@
 The first digit of the number is guaranteed to be non-zero by adding 10 to the modulus (so the first two digits range from 10 through to 99).
 For companies the last 9 digits are identical to their existing Australian Company Number (CAN) which includes a single trailing check digit.
 For other entities the digits are randomly allocated but are guaranteed to fail the CAN check. This allows the Australian Securities and Investment Commission (ASIC) to continue allocating CAN during a transition period. The valid characters are numeric digits 0-9.</t>
-  </si>
-  <si>
-    <t>8 or 10 digits</t>
   </si>
   <si>
     <t>20 digits
@@ -1897,9 +1872,6 @@
     <t>false</t>
   </si>
   <si>
-    <t>RegEx: DK[0-9]{8}([0-9]{2})?</t>
-  </si>
-  <si>
     <t>0230</t>
   </si>
   <si>
@@ -1981,6 +1953,38 @@
   </si>
   <si>
     <t>RegEx: [0-9]{9}([0-9]{2})?</t>
+  </si>
+  <si>
+    <t>The Danish Business Authority - P-number (DK:P)</t>
+  </si>
+  <si>
+    <t>XXXXXXXXXX
+10 digits eg. 1234567890</t>
+  </si>
+  <si>
+    <t>RegEx: [0-9]{10}</t>
+  </si>
+  <si>
+    <t>A P-number that represents a production unit.</t>
+  </si>
+  <si>
+    <t>The Danish Business Authority - CVR-number (DK:CVR)</t>
+  </si>
+  <si>
+    <t>XXXXXXXX
+8 digits eg. 12345678</t>
+  </si>
+  <si>
+    <t>8 characters, no space or other separator</t>
+  </si>
+  <si>
+    <t>RegEx: [1-9][0-9]{7}</t>
+  </si>
+  <si>
+    <t>A CVR number uniquely identifies a legal entity. CVR stands for “Central Business Register” and contains information about all registered companies in Denmark.</t>
+  </si>
+  <si>
+    <t>The Danish Business Authority - SE-number (DK:SE)</t>
   </si>
 </sst>
 </file>
@@ -2770,10 +2774,10 @@
   <dimension ref="A1:AMN102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,7 +2791,7 @@
     <col min="7" max="7" width="11.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="62.42578125" style="9" customWidth="1"/>
     <col min="11" max="11" width="45.140625" style="9" customWidth="1"/>
     <col min="12" max="12" width="30.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30.5703125" style="10" customWidth="1"/>
@@ -2813,16 +2817,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>5</v>
@@ -2831,16 +2835,16 @@
         <v>6</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
@@ -2863,25 +2867,25 @@
         <v>13</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -2904,22 +2908,22 @@
         <v>13</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2942,22 +2946,22 @@
         <v>25</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="150" x14ac:dyDescent="0.25">
@@ -2980,25 +2984,25 @@
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="O5" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="105" x14ac:dyDescent="0.25">
@@ -3021,25 +3025,25 @@
         <v>13</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>42</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -3062,28 +3066,28 @@
         <v>13</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="195" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
@@ -3094,1247 +3098,1253 @@
         <v>45</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>46</v>
+        <v>555</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>47</v>
+        <v>343</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>371</v>
+        <v>556</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>32</v>
+        <v>345</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>434</v>
+        <v>557</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>558</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="D9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>52</v>
-      </c>
       <c r="E9" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>32</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="O9" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="210" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>58</v>
-      </c>
       <c r="G10" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>32</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="O10" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="G11" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>32</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="O11" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>68</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>32</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="O12" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>32</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="O13" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="240" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="F14" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="G14" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>80</v>
-      </c>
       <c r="L14" s="10" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="O14" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="150" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="K15" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="O15" s="10" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>339</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>338</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="N15" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="O15" s="10" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="B16" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>83</v>
+        <v>559</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>83</v>
+        <v>343</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>375</v>
+        <v>560</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>383</v>
+        <v>561</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>538</v>
+        <v>562</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>563</v>
       </c>
       <c r="O16" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="17" spans="1:15 1028:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>499</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>503</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>500</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>505</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>32</v>
       </c>
       <c r="O17" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="18" spans="1:15 1028:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="F18" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>89</v>
-      </c>
       <c r="G18" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="O18" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="19" spans="1:15 1028:1028" ht="225" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>94</v>
-      </c>
       <c r="F19" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="K19" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="O19" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="20" spans="1:15 1028:1028" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="F20" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J20" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="O20" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="21" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="G21" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J21" s="9" t="s">
         <v>104</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J21" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>32</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="O21" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="22" spans="1:15 1028:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="E22" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>112</v>
-      </c>
       <c r="F22" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="N22" s="7" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="O22" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="23" spans="1:15 1028:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="F23" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="K23" s="9" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="O23" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="24" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>45</v>
       </c>
       <c r="D24" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="K24" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>349</v>
-      </c>
       <c r="M24" s="10" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="O24" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="25" spans="1:15 1028:1028" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="O25" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="26" spans="1:15 1028:1028" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="E26" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="F26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>120</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="K26" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="O26" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="27" spans="1:15 1028:1028" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>355</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="G27" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J27" s="9" t="s">
         <v>356</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>358</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>360</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L27" s="11"/>
       <c r="M27" s="11" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="O27" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN27" s="7"/>
     </row>
     <row r="28" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="K28" s="9" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="L28" s="11"/>
       <c r="M28" s="11" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN28" s="7"/>
     </row>
     <row r="29" spans="1:15 1028:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
       <c r="N29" s="7" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
       <c r="O29" s="10" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="AMN29" s="7"/>
     </row>
     <row r="30" spans="1:15 1028:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="K30" s="9" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="L30" s="11"/>
       <c r="M30" s="10" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="O30" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN30" s="7"/>
     </row>
     <row r="31" spans="1:15 1028:1028" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="K31" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L31" s="11" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN31" s="7"/>
     </row>
     <row r="32" spans="1:15 1028:1028" ht="255" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="L32" s="11"/>
       <c r="M32" s="10" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="O32" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN32" s="7"/>
     </row>
     <row r="33" spans="1:1028" ht="105" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="L33" s="11"/>
       <c r="M33" s="10" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="O33" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN33" s="7"/>
     </row>
     <row r="34" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="L34" s="11"/>
       <c r="M34" s="10" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN34" s="7"/>
     </row>
     <row r="35" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="E35" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>457</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="K35" s="9" t="s">
         <v>479</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>463</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>484</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>485</v>
       </c>
       <c r="L35" s="11"/>
       <c r="M35" s="10" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN35" s="7"/>
     </row>
     <row r="36" spans="1:1028" ht="150" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="K36" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L36" s="11"/>
       <c r="M36" s="10" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="O36" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN36" s="7"/>
     </row>
     <row r="37" spans="1:1028" ht="240" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>29</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="K37" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L37" s="11"/>
       <c r="M37" s="10" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="O37" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN37" s="7"/>
     </row>
     <row r="38" spans="1:1028" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="K38" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L38" s="11"/>
       <c r="M38" s="10" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="O38" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN38" s="7"/>
     </row>
     <row r="39" spans="1:1028" ht="180" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="F39" s="12" t="s">
+        <v>536</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="J39" s="9" t="s">
         <v>543</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>550</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L39" s="11"/>
       <c r="N39" s="7" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="O39" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN39" s="7"/>
     </row>
     <row r="40" spans="1:1028" ht="90" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="K40" s="9" t="s">
         <v>32</v>
       </c>
       <c r="L40" s="11"/>
       <c r="N40" s="7" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="O40" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="AMN40" s="7"/>
     </row>
     <row r="41" spans="1:1028" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H41" s="16" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="I41" s="18">
         <v>45260</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K41" s="19" t="s">
         <v>32</v>
@@ -4342,10 +4352,10 @@
       <c r="L41" s="17"/>
       <c r="M41" s="17"/>
       <c r="N41" s="15" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="O41" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P41" s="15"/>
       <c r="Q41" s="15"/>
@@ -5362,28 +5372,28 @@
     </row>
     <row r="42" spans="1:1028" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F42" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="I42" s="18">
         <v>45260</v>
@@ -5391,14 +5401,14 @@
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
       <c r="L42" s="17" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="M42" s="17" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="N42" s="15"/>
       <c r="O42" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P42" s="15"/>
       <c r="Q42" s="15"/>
@@ -6415,28 +6425,28 @@
     </row>
     <row r="43" spans="1:1028" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F43" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H43" s="16" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="I43" s="18">
         <v>45260</v>
@@ -6444,14 +6454,14 @@
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
       <c r="L43" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M43" s="17" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="N43" s="15"/>
       <c r="O43" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P43" s="15"/>
       <c r="Q43" s="15"/>
@@ -7468,28 +7478,28 @@
     </row>
     <row r="44" spans="1:1028" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F44" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H44" s="16" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="I44" s="18">
         <v>45260</v>
@@ -7497,14 +7507,14 @@
       <c r="J44" s="19"/>
       <c r="K44" s="19"/>
       <c r="L44" s="17" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="15" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="O44" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P44" s="15"/>
       <c r="Q44" s="15"/>
@@ -8521,43 +8531,43 @@
     </row>
     <row r="45" spans="1:1028" s="20" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E45" s="15"/>
       <c r="F45" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H45" s="16" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="I45" s="18">
         <v>45070</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="K45" s="19"/>
       <c r="L45" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M45" s="17" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="N45" s="15"/>
       <c r="O45" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P45" s="15"/>
       <c r="Q45" s="15"/>
@@ -9574,28 +9584,28 @@
     </row>
     <row r="46" spans="1:1028" s="20" customFormat="1" ht="285" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F46" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H46" s="16" t="s">
-        <v>500</v>
+        <v>494</v>
       </c>
       <c r="I46" s="18">
         <v>45070</v>
@@ -9603,16 +9613,16 @@
       <c r="J46" s="19"/>
       <c r="K46" s="19"/>
       <c r="L46" s="17" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="M46" s="17" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="N46" s="15" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="O46" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
@@ -10629,45 +10639,45 @@
     </row>
     <row r="47" spans="1:1028" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F47" s="16" t="s">
         <v>13</v>
       </c>
       <c r="G47" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="I47" s="18">
         <v>45070</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K47" s="19"/>
       <c r="L47" s="17"/>
       <c r="M47" s="17" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="N47" s="15" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="O47" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
@@ -11684,365 +11694,365 @@
     </row>
     <row r="48" spans="1:1028" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M48" s="10" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="N48" s="7" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="O48" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="49" spans="1:1027" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D49" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>154</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="M49" s="10" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="O49" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="50" spans="1:1027" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E50"/>
       <c r="F50" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M50" s="10" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="N50" s="7" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="O50" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="51" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="N51" s="7" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="O51" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="52" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D52" s="7" t="s">
-        <v>166</v>
       </c>
       <c r="F52" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="L52" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="O52" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="53" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E53"/>
       <c r="F53" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="M53" s="10" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="N53" s="7" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="O53" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="54" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F54" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="O54" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="55" spans="1:1027" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F55" s="8" t="s">
         <v>13</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="H55" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="M55" s="10" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="N55" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="O55" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="56" spans="1:1027" ht="75" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="O56" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="57" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E57"/>
       <c r="F57" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="N57" s="7" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="O57" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="58" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O58" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="59" spans="1:1027" s="20" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G59" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H59" s="21" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="I59" s="18">
         <v>45260</v>
@@ -12052,10 +12062,10 @@
       <c r="L59" s="17"/>
       <c r="M59" s="17"/>
       <c r="N59" s="15" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="O59" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P59" s="15"/>
       <c r="Q59" s="15"/>
@@ -13072,826 +13082,826 @@
     </row>
     <row r="60" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D60" s="7" t="s">
         <v>193</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>196</v>
       </c>
       <c r="E60"/>
       <c r="F60" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O60" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="61" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D61" s="7" t="s">
         <v>197</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D61" s="7" t="s">
-        <v>200</v>
       </c>
       <c r="E61"/>
       <c r="F61" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O61" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="62" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D62" s="7" t="s">
         <v>201</v>
-      </c>
-      <c r="B62" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="E62"/>
       <c r="F62" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O62" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="63" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E63"/>
       <c r="F63" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O63" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="64" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D64" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="B64" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="D64" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="E64"/>
       <c r="F64" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O64" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D65" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D65" s="7" t="s">
-        <v>215</v>
       </c>
       <c r="E65"/>
       <c r="F65" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O65" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D66" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="D66" s="7" t="s">
-        <v>219</v>
-      </c>
       <c r="F66" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O66" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D67" s="7" t="s">
         <v>220</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="D67" s="7" t="s">
-        <v>223</v>
       </c>
       <c r="E67"/>
       <c r="F67" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O67" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>224</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>227</v>
       </c>
       <c r="E68"/>
       <c r="F68" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O68" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E69"/>
       <c r="F69" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O69" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D70" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>232</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="E70"/>
       <c r="F70" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O70" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D71" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="B71" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>238</v>
       </c>
       <c r="E71"/>
       <c r="F71" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O71" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D72" s="7" t="s">
         <v>239</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>242</v>
       </c>
       <c r="E72"/>
       <c r="F72" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O72" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D73" s="7" t="s">
         <v>243</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>246</v>
       </c>
       <c r="E73"/>
       <c r="F73" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O73" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D74" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>249</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>250</v>
       </c>
       <c r="E74"/>
       <c r="F74" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O74" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E75"/>
       <c r="F75" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O75" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
+        <v>251</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D76" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>255</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>257</v>
       </c>
       <c r="E76"/>
       <c r="F76" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O76" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>258</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>261</v>
       </c>
       <c r="E77"/>
       <c r="F77" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O77" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="D78" s="7" t="s">
         <v>262</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>265</v>
       </c>
       <c r="E78"/>
       <c r="F78" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O78" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="D79" s="7" t="s">
         <v>266</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>267</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>269</v>
       </c>
       <c r="E79"/>
       <c r="F79" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O79" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="D80" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="E80"/>
       <c r="F80" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O80" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="81" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A81" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D81" s="7" t="s">
         <v>274</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>277</v>
       </c>
       <c r="E81"/>
       <c r="F81" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O81" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="82" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D82" s="7" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E82"/>
       <c r="F82" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O82" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="83" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A83" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D83" s="7" t="s">
         <v>281</v>
-      </c>
-      <c r="B83" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>284</v>
       </c>
       <c r="E83"/>
       <c r="F83" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O83" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="84" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A84" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D84" s="7" t="s">
         <v>285</v>
-      </c>
-      <c r="B84" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>288</v>
       </c>
       <c r="E84"/>
       <c r="F84" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O84" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="85" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
+        <v>286</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D85" s="7" t="s">
         <v>289</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>292</v>
       </c>
       <c r="E85"/>
       <c r="F85" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G85" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="I85" s="3"/>
       <c r="O85" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="86" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D86" s="7" t="s">
         <v>293</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>296</v>
       </c>
       <c r="E86"/>
       <c r="F86" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="I86" s="3"/>
       <c r="O86" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="87" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="D87" s="7" t="s">
         <v>297</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>300</v>
       </c>
       <c r="E87"/>
       <c r="F87" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="I87" s="3"/>
       <c r="O87" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="88" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D88" s="7" t="s">
         <v>301</v>
-      </c>
-      <c r="B88" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>304</v>
       </c>
       <c r="E88"/>
       <c r="F88" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G88" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O88" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="89" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="D89" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="B89" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>308</v>
-      </c>
       <c r="F89" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G89" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O89" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="90" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="D90" s="7" t="s">
         <v>309</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>312</v>
       </c>
       <c r="E90"/>
       <c r="F90" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G90" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="I90" s="4"/>
       <c r="O90" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="91" spans="1:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="D91" s="7" t="s">
         <v>313</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>316</v>
       </c>
       <c r="E91"/>
       <c r="F91" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O91" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="92" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="F92" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="B92" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>320</v>
-      </c>
       <c r="G92" s="10" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I92" s="3"/>
       <c r="N92" s="7" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="O92" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="93" spans="1:1027" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C93" s="15" t="s">
         <v>17</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E93" s="15"/>
       <c r="F93" s="16" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G93" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H93" s="16" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="I93" s="22">
         <v>45138</v>
@@ -13902,7 +13912,7 @@
       <c r="M93" s="17"/>
       <c r="N93" s="15"/>
       <c r="O93" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P93" s="15"/>
       <c r="Q93" s="15"/>
@@ -14919,45 +14929,45 @@
     </row>
     <row r="94" spans="1:1027" s="20" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="B94" s="15" t="s">
+        <v>324</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="E94" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="B94" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D94" s="15" t="s">
-        <v>328</v>
-      </c>
-      <c r="E94" s="15" t="s">
-        <v>329</v>
-      </c>
       <c r="F94" s="16" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G94" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H94" s="16" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="I94" s="22">
         <v>45291</v>
       </c>
       <c r="J94" s="19" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K94" s="19"/>
       <c r="L94" s="17" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="M94" s="17" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="N94" s="15"/>
       <c r="O94" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P94" s="15"/>
       <c r="Q94" s="15"/>
@@ -15974,49 +15984,49 @@
     </row>
     <row r="95" spans="1:1027" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C95" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O95" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="96" spans="1:1027" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C96" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E96" s="15"/>
       <c r="F96" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G96" s="17" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="H96" s="16" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="I96" s="22">
         <v>45138</v>
@@ -16026,10 +16036,10 @@
       <c r="L96" s="17"/>
       <c r="M96" s="17"/>
       <c r="N96" s="15" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="O96" s="17" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="P96" s="15"/>
       <c r="Q96" s="15"/>
@@ -17046,25 +17056,25 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="O97" s="10" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>